<commit_message>
Added Code for Product module
</commit_message>
<xml_diff>
--- a/GUISeleniumFramework/testdata/testScriptdata.xlsx
+++ b/GUISeleniumFramework/testdata/testScriptdata.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20400"/>
-  <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B66EEE0E-7793-4D98-9BEE-A78371A6E345}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rushm\git\DoliBarr_Framework_New\GUISeleniumFramework\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11620" windowHeight="6330" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11625" windowHeight="6330" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="3" r:id="rId1"/>
     <sheet name="org" sheetId="1" r:id="rId2"/>
-    <sheet name="product" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="2" state="hidden" r:id="rId4"/>
+    <sheet name="PRODUCTS" sheetId="5" r:id="rId3"/>
+    <sheet name="SERVICES" sheetId="6" r:id="rId4"/>
+    <sheet name="product" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="2" state="hidden" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E15"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="152">
   <si>
     <t>TC_ID</t>
   </si>
@@ -444,12 +449,48 @@
   </si>
   <si>
     <t>faceBook_kdd</t>
+  </si>
+  <si>
+    <t>ProductRef</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Oven</t>
+  </si>
+  <si>
+    <t>modifyProductTest</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>LG_Oven</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>mg</t>
+  </si>
+  <si>
+    <t>deleteServiceTest</t>
+  </si>
+  <si>
+    <t>Car_Service</t>
+  </si>
+  <si>
+    <t>Car Wash</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -797,22 +838,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{618505B5-BC18-40DF-B31F-D9D1863412AA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="2" max="2" width="30.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -827,7 +868,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>115</v>
       </c>
@@ -840,14 +881,14 @@
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -862,7 +903,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>116</v>
       </c>
@@ -875,14 +916,14 @@
       <c r="D5" s="3"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -899,7 +940,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>127</v>
       </c>
@@ -920,21 +961,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A26" zoomScale="130" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.81640625" customWidth="1"/>
-    <col min="3" max="3" width="18.26953125" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -947,7 +988,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -960,7 +1001,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -977,7 +1018,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>110</v>
       </c>
@@ -994,7 +1035,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1008,7 +1049,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>111</v>
       </c>
@@ -1022,7 +1063,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1034,7 +1075,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>115</v>
       </c>
@@ -1052,20 +1093,141 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B6E95A9-5958-495C-AC30-1DA708189BFF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>133</v>
       </c>
@@ -1073,7 +1235,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>135</v>
       </c>
@@ -1081,7 +1243,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>135</v>
       </c>
@@ -1089,7 +1251,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>135</v>
       </c>
@@ -1102,21 +1264,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7004AA42-F8FF-45C9-AB36-1F51EDB304F0}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1124,7 +1286,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1132,7 +1294,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1140,7 +1302,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1148,7 +1310,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1156,7 +1318,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1164,7 +1326,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1172,7 +1334,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1180,7 +1342,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1188,7 +1350,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1196,7 +1358,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1204,7 +1366,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -1212,7 +1374,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -1220,7 +1382,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1228,7 +1390,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1236,7 +1398,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1244,7 +1406,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1252,7 +1414,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -1260,7 +1422,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -1268,7 +1430,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -1276,7 +1438,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -1284,7 +1446,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
@@ -1292,7 +1454,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>14</v>
       </c>
@@ -1300,7 +1462,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>14</v>
       </c>
@@ -1308,7 +1470,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
@@ -1316,7 +1478,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>14</v>
       </c>
@@ -1324,7 +1486,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>14</v>
       </c>
@@ -1332,7 +1494,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
@@ -1340,7 +1502,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>14</v>
       </c>
@@ -1348,7 +1510,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>14</v>
       </c>
@@ -1356,7 +1518,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>14</v>
       </c>
@@ -1364,7 +1526,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>14</v>
       </c>
@@ -1372,7 +1534,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>14</v>
       </c>
@@ -1380,7 +1542,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>14</v>
       </c>
@@ -1388,7 +1550,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>14</v>
       </c>
@@ -1396,7 +1558,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>14</v>
       </c>
@@ -1404,7 +1566,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>14</v>
       </c>
@@ -1412,7 +1574,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>14</v>
       </c>
@@ -1420,7 +1582,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>14</v>
       </c>
@@ -1428,7 +1590,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>14</v>
       </c>
@@ -1436,7 +1598,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>14</v>
       </c>
@@ -1444,7 +1606,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>14</v>
       </c>
@@ -1452,7 +1614,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>14</v>
       </c>
@@ -1460,7 +1622,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>14</v>
       </c>
@@ -1468,7 +1630,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>14</v>
       </c>
@@ -1476,7 +1638,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>14</v>
       </c>
@@ -1484,7 +1646,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>14</v>
       </c>
@@ -1492,7 +1654,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>14</v>
       </c>
@@ -1500,7 +1662,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>14</v>
       </c>
@@ -1508,7 +1670,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>14</v>
       </c>
@@ -1516,7 +1678,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>58</v>
       </c>
@@ -1524,7 +1686,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>58</v>
       </c>
@@ -1532,7 +1694,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>58</v>
       </c>
@@ -1540,7 +1702,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>58</v>
       </c>
@@ -1548,7 +1710,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>58</v>
       </c>
@@ -1556,7 +1718,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>58</v>
       </c>
@@ -1564,7 +1726,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>58</v>
       </c>
@@ -1572,7 +1734,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>58</v>
       </c>
@@ -1580,7 +1742,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>58</v>
       </c>
@@ -1588,7 +1750,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>58</v>
       </c>
@@ -1596,7 +1758,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>58</v>
       </c>
@@ -1604,7 +1766,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>58</v>
       </c>
@@ -1612,7 +1774,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>58</v>
       </c>
@@ -1620,7 +1782,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>58</v>
       </c>
@@ -1628,7 +1790,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>58</v>
       </c>
@@ -1636,7 +1798,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>58</v>
       </c>
@@ -1644,7 +1806,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>58</v>
       </c>
@@ -1652,7 +1814,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>58</v>
       </c>
@@ -1660,7 +1822,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>58</v>
       </c>
@@ -1668,7 +1830,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>58</v>
       </c>
@@ -1676,7 +1838,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>58</v>
       </c>
@@ -1684,7 +1846,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>58</v>
       </c>
@@ -1692,7 +1854,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>58</v>
       </c>
@@ -1700,7 +1862,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>58</v>
       </c>
@@ -1708,7 +1870,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>58</v>
       </c>
@@ -1716,7 +1878,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>58</v>
       </c>
@@ -1724,7 +1886,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>58</v>
       </c>
@@ -1732,7 +1894,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>58</v>
       </c>
@@ -1740,7 +1902,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>58</v>
       </c>
@@ -1748,7 +1910,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>58</v>
       </c>
@@ -1756,7 +1918,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>58</v>
       </c>
@@ -1764,7 +1926,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>58</v>
       </c>
@@ -1772,7 +1934,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>58</v>
       </c>
@@ -1780,7 +1942,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>58</v>
       </c>
@@ -1788,7 +1950,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>58</v>
       </c>
@@ -1796,7 +1958,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>58</v>
       </c>
@@ -1804,7 +1966,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>58</v>
       </c>
@@ -1812,7 +1974,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>58</v>
       </c>
@@ -1820,7 +1982,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>58</v>
       </c>
@@ -1828,7 +1990,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>58</v>
       </c>
@@ -1836,7 +1998,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>58</v>
       </c>
@@ -1844,7 +2006,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>58</v>
       </c>
@@ -1852,7 +2014,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>58</v>
       </c>
@@ -1860,7 +2022,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>58</v>
       </c>
@@ -1868,7 +2030,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>58</v>
       </c>
@@ -1876,7 +2038,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>58</v>
       </c>
@@ -1884,7 +2046,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>58</v>
       </c>
@@ -1892,7 +2054,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>58</v>
       </c>
@@ -1900,7 +2062,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>58</v>
       </c>
@@ -1908,7 +2070,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>58</v>
       </c>

</xml_diff>